<commit_message>
add conversions for generali
</commit_message>
<xml_diff>
--- a/public/fonduri conversie reusita/Conversia/20241130_pII_inv_det.xlsx
+++ b/public/fonduri conversie reusita/Conversia/20241130_pII_inv_det.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,21 +436,757 @@
         <v/>
       </c>
       <c r="D2" t="str">
-        <v>c. Obligatiuni corporative tranzactionate</v>
+        <v>4,302,514,060.98</v>
       </c>
       <c r="E2" t="str">
-        <v>b. Obligatiuni emise de administratia publica locala</v>
+        <v>31.35%</v>
       </c>
       <c r="F2" t="str">
         <v/>
       </c>
       <c r="G2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Adidas AG</v>
+      </c>
+      <c r="B3" t="str">
+        <v>DE000A1EWWW0</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v>56,323,473.59</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0.41%</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Aquila Part Prod Com SA</v>
+      </c>
+      <c r="B4" t="str">
+        <v>RO7066ZEA1R9</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v>32,461,802.36</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0.24%</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Axa SA</v>
+      </c>
+      <c r="B5" t="str">
+        <v>FR0000120628</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>80,430,767.28</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0.59%</v>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Banca Transilvania SA</v>
+      </c>
+      <c r="B6" t="str">
+        <v>ROTLVAACNOR1</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>631,531,243.20</v>
+      </c>
+      <c r="E6" t="str">
+        <v>4.60%</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Basf Se</v>
+      </c>
+      <c r="B7" t="str">
+        <v>DE000BASF111</v>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v>14,636,066.69</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0.11%</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BNP Paribas</v>
+      </c>
+      <c r="B8" t="str">
+        <v>FR0000131104</v>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v>17,317,297.85</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0.13%</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>BRD - Groupe Societe Generale SA</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ROBRDBACNOR2</v>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v>229,434,706.98</v>
+      </c>
+      <c r="E9" t="str">
+        <v>1.67%</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Capgemini SA</v>
+      </c>
+      <c r="B10" t="str">
+        <v>FR0000125338</v>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <v>71,171,863.07</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0.52%</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Compagnie de Saint - Gobain</v>
+      </c>
+      <c r="B11" t="str">
+        <v>FR0000125007</v>
+      </c>
+      <c r="C11" t="str">
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <v>74,284,893.69</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0.54%</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Daimler Truck Holding AG</v>
+      </c>
+      <c r="B12" t="str">
+        <v>DE000DTR0CK8</v>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <v>10,287,767.23</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0.07%</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>DHL Group</v>
+      </c>
+      <c r="B13" t="str">
+        <v>DE0005552004</v>
+      </c>
+      <c r="C13" t="str">
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <v>26,353,492.91</v>
+      </c>
+      <c r="E13" t="str">
+        <v>0.19%</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Digi Communications NV</v>
+      </c>
+      <c r="B14" t="str">
+        <v>NL0012294474</v>
+      </c>
+      <c r="C14" t="str">
+        <v/>
+      </c>
+      <c r="D14" t="str">
+        <v>166,294,400.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>1.21%</v>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Electrica SA</v>
+      </c>
+      <c r="B15" t="str">
+        <v>ROELECACNOR5</v>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v>145,554,828.78</v>
+      </c>
+      <c r="E15" t="str">
+        <v>1.06%</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Fresenius SE &amp; CO</v>
+      </c>
+      <c r="B16" t="str">
+        <v>DE0005785604</v>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v>15,944,479.79</v>
+      </c>
+      <c r="E16" t="str">
+        <v>0.12%</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Hidroelectrica SA</v>
+      </c>
+      <c r="B17" t="str">
+        <v>RO4Q0Z5RO1B6</v>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v>637,761,369.00</v>
+      </c>
+      <c r="E17" t="str">
+        <v>4.65%</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Infineon Technologies Ag</v>
+      </c>
+      <c r="B18" t="str">
+        <v>DE0006231004</v>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v>61,775,941.79</v>
+      </c>
+      <c r="E18" t="str">
+        <v>0.45%</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>LVMH Moet Hennessy Louis Vuitton SA</v>
+      </c>
+      <c r="B19" t="str">
+        <v>FR0000121014</v>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v>94,336,326.68</v>
+      </c>
+      <c r="E19" t="str">
+        <v>0.69%</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Med Life SA</v>
+      </c>
+      <c r="B20" t="str">
+        <v>ROMEDLACNOR6</v>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v>141,428,610.40</v>
+      </c>
+      <c r="E20" t="str">
+        <v>1.03%</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Mercedes Benz Group AG</v>
+      </c>
+      <c r="B21" t="str">
+        <v>DE0007100000</v>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <v>33,695,144.58</v>
+      </c>
+      <c r="E21" t="str">
+        <v>0.25%</v>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Nuclearelectrica SA</v>
+      </c>
+      <c r="B22" t="str">
+        <v>ROSNNEACNOR8</v>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <v>118,513,023.70</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0.86%</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>OMV Petrom SA</v>
+      </c>
+      <c r="B23" t="str">
+        <v>ROSNPPACNOR9</v>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v>593,127,471.07</v>
+      </c>
+      <c r="E23" t="str">
+        <v>4.32%</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Premier Energy PLC</v>
+      </c>
+      <c r="B24" t="str">
+        <v>CY0200900914</v>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <v>47,513,963.84</v>
+      </c>
+      <c r="E24" t="str">
+        <v>0.35%</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Romgaz SA</v>
+      </c>
+      <c r="B25" t="str">
+        <v>ROSNGNACNOR3</v>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <v>397,492,394.72</v>
+      </c>
+      <c r="E25" t="str">
+        <v>2.90%</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>SAP SE</v>
+      </c>
+      <c r="B26" t="str">
+        <v>DE0007164600</v>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <v>104,102,888.52</v>
+      </c>
+      <c r="E26" t="str">
+        <v>0.76%</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Schneider Electric</v>
+      </c>
+      <c r="B27" t="str">
+        <v>FR0000121972</v>
+      </c>
+      <c r="C27" t="str">
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <v>117,994,117.96</v>
+      </c>
+      <c r="E27" t="str">
+        <v>0.86%</v>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Siemens AG</v>
+      </c>
+      <c r="B28" t="str">
+        <v>DE0007236101</v>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v>59,041,050.62</v>
+      </c>
+      <c r="E28" t="str">
+        <v>0.43%</v>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+      <c r="G28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Sphera Franchise Group SA</v>
+      </c>
+      <c r="B29" t="str">
+        <v>ROSFGPACNOR4</v>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v>18,442,681.20</v>
+      </c>
+      <c r="E29" t="str">
+        <v>0.13%</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>TotalEnergies SE</v>
+      </c>
+      <c r="B30" t="str">
+        <v>FR0000120271</v>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v>109,434,012.48</v>
+      </c>
+      <c r="E30" t="str">
+        <v>0.80%</v>
+      </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Transelectrica SA</v>
+      </c>
+      <c r="B31" t="str">
+        <v>ROTSELACNOR9</v>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v>51,515,987.25</v>
+      </c>
+      <c r="E31" t="str">
+        <v>0.38%</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Transgaz SA</v>
+      </c>
+      <c r="B32" t="str">
+        <v>ROTGNTACNOR8</v>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v>76,392,335.25</v>
+      </c>
+      <c r="E32" t="str">
+        <v>0.56%</v>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Vinci SA</v>
+      </c>
+      <c r="B33" t="str">
+        <v>FR0000125486</v>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v>61,861,245.70</v>
+      </c>
+      <c r="E33" t="str">
+        <v>0.45%</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Volkswagen AG</v>
+      </c>
+      <c r="B34" t="str">
+        <v>DE0007664039</v>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v>6,058,412.80</v>
+      </c>
+      <c r="E34" t="str">
+        <v>0.04%</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+      <c r="G34" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>